<commit_message>
products import data on create
</commit_message>
<xml_diff>
--- a/public/excel/import.xlsx
+++ b/public/excel/import.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="209">
   <si>
     <t>crd_product</t>
   </si>
@@ -448,7 +448,7 @@
     <t>TCl-F4</t>
   </si>
   <si>
-    <t xml:space="preserve">ФОТО 1, </t>
+    <t>BN8830_1.jpg,BN8830_2.jpg</t>
   </si>
   <si>
     <t>BN8830</t>
@@ -478,6 +478,24 @@
     <t>(160x200)</t>
   </si>
   <si>
+    <t>BN8830 description it</t>
+  </si>
+  <si>
+    <t>BN8830 descripton en</t>
+  </si>
+  <si>
+    <t>BN8830 descr ru</t>
+  </si>
+  <si>
+    <t>BNLettoDOUBLE descr it</t>
+  </si>
+  <si>
+    <t>BNLettoDOUBLE descr en</t>
+  </si>
+  <si>
+    <t>BNLettoDOUBLE descr ru</t>
+  </si>
+  <si>
     <t>L192 P217 H130 (160x200)</t>
   </si>
   <si>
@@ -487,13 +505,13 @@
     <t>3,4m²</t>
   </si>
   <si>
-    <t>ФОТО 2</t>
-  </si>
-  <si>
-    <t>ФОТО 3</t>
-  </si>
-  <si>
-    <t>ФОТО 1</t>
+    <t>BN8830_3.jpg</t>
+  </si>
+  <si>
+    <t>BN8830_4.jpg</t>
+  </si>
+  <si>
+    <t>BN8831_1.jpg</t>
   </si>
   <si>
     <t>BN8831</t>
@@ -511,6 +529,15 @@
     <t>(180x200)</t>
   </si>
   <si>
+    <t>BN8831 description it</t>
+  </si>
+  <si>
+    <t>BN8831 descripton en</t>
+  </si>
+  <si>
+    <t>BN8831 descr ru</t>
+  </si>
+  <si>
     <t>L211 P217 H130 (180x200)</t>
   </si>
   <si>
@@ -518,13 +545,118 @@
   </si>
   <si>
     <t>3,8m²</t>
+  </si>
+  <si>
+    <t>BN8831_2.jpg</t>
+  </si>
+  <si>
+    <t>BN8831_3.jpg</t>
+  </si>
+  <si>
+    <t>BN8830_1.jpg</t>
+  </si>
+  <si>
+    <t>BN8834</t>
+  </si>
+  <si>
+    <t>BNLettoDOUBLE2</t>
+  </si>
+  <si>
+    <t>Letto2</t>
+  </si>
+  <si>
+    <t>Bed2</t>
+  </si>
+  <si>
+    <t>Кровать2</t>
+  </si>
+  <si>
+    <t>Letto 170</t>
+  </si>
+  <si>
+    <t>Bed 170</t>
+  </si>
+  <si>
+    <t>Кровать 170</t>
+  </si>
+  <si>
+    <t>(170x200)</t>
+  </si>
+  <si>
+    <t>BN8834 description it</t>
+  </si>
+  <si>
+    <t>BN8834 descripton en</t>
+  </si>
+  <si>
+    <t>BN8834 descr ru</t>
+  </si>
+  <si>
+    <t>BNLettoDOUBLE2 descr it</t>
+  </si>
+  <si>
+    <t>BNLettoDOUBLE2 descr en</t>
+  </si>
+  <si>
+    <t>BNLettoDOUBLE2 descr ru</t>
+  </si>
+  <si>
+    <t>BN8830_2.jpg,BN8830_3.jpg</t>
+  </si>
+  <si>
+    <t>BN8835</t>
+  </si>
+  <si>
+    <t>Letto 190</t>
+  </si>
+  <si>
+    <t>Bed 190</t>
+  </si>
+  <si>
+    <t>Кровать 190</t>
+  </si>
+  <si>
+    <t>(190x200)</t>
+  </si>
+  <si>
+    <t>BN8835 description it</t>
+  </si>
+  <si>
+    <t>BN8835 descripton en</t>
+  </si>
+  <si>
+    <t>BN8835 descr ru</t>
+  </si>
+  <si>
+    <t>BN8836</t>
+  </si>
+  <si>
+    <t>Letto 210</t>
+  </si>
+  <si>
+    <t>Bed 210</t>
+  </si>
+  <si>
+    <t>Кровать 210</t>
+  </si>
+  <si>
+    <t>(210x200)</t>
+  </si>
+  <si>
+    <t>BN8836 description it</t>
+  </si>
+  <si>
+    <t>BN8836 descripton en</t>
+  </si>
+  <si>
+    <t>BN8836 descr ru</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -570,8 +702,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,8 +751,14 @@
         <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -706,11 +849,25 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -809,7 +966,7 @@
     <xf borderId="9" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="6" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -828,13 +985,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="6" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -856,6 +1019,69 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="7" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="9" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="7" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="7" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="7" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -876,6 +1102,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="25.29"/>
+    <col customWidth="1" min="5" max="5" width="18.86"/>
+    <col customWidth="1" min="35" max="35" width="22.43"/>
+    <col customWidth="1" min="36" max="36" width="18.14"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -1507,20 +1739,32 @@
         <v>150</v>
       </c>
       <c r="AH5" s="40"/>
-      <c r="AI5" s="42"/>
-      <c r="AJ5" s="42"/>
-      <c r="AK5" s="40"/>
-      <c r="AL5" s="42"/>
-      <c r="AM5" s="42"/>
-      <c r="AN5" s="40"/>
+      <c r="AI5" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ5" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK5" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL5" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM5" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN5" s="43" t="s">
+        <v>156</v>
+      </c>
       <c r="AO5" s="39" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="AP5" s="39" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="AQ5" s="39" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="AR5" s="39">
         <v>5702.0</v>
@@ -1563,84 +1807,84 @@
       <c r="A6" s="35">
         <v>2.0</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>154</v>
+      <c r="B6" s="44" t="s">
+        <v>160</v>
       </c>
       <c r="C6" s="37"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="43"/>
-      <c r="X6" s="43"/>
-      <c r="Y6" s="43"/>
-      <c r="Z6" s="43"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="43"/>
-      <c r="AC6" s="43"/>
-      <c r="AD6" s="43"/>
-      <c r="AE6" s="43"/>
-      <c r="AF6" s="43"/>
-      <c r="AG6" s="43"/>
-      <c r="AH6" s="43"/>
-      <c r="AK6" s="43"/>
-      <c r="AN6" s="43"/>
-      <c r="AO6" s="43"/>
-      <c r="AP6" s="43"/>
-      <c r="AQ6" s="43"/>
-      <c r="AR6" s="43"/>
-      <c r="AS6" s="43"/>
-      <c r="AT6" s="43"/>
-      <c r="AU6" s="43"/>
-      <c r="AV6" s="43"/>
-      <c r="AW6" s="43"/>
-      <c r="AX6" s="43"/>
-      <c r="AY6" s="43"/>
-      <c r="AZ6" s="43"/>
-      <c r="BA6" s="43"/>
-      <c r="BB6" s="43"/>
-      <c r="BC6" s="43"/>
-      <c r="BD6" s="43"/>
-      <c r="BE6" s="43"/>
-      <c r="BF6" s="43"/>
-      <c r="BG6" s="43"/>
-      <c r="BH6" s="43"/>
-      <c r="BI6" s="43"/>
-      <c r="BJ6" s="43"/>
-      <c r="BK6" s="43"/>
-      <c r="BL6" s="43"/>
-      <c r="BM6" s="43"/>
-      <c r="BN6" s="43"/>
-      <c r="BO6" s="43"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="45"/>
+      <c r="AB6" s="45"/>
+      <c r="AC6" s="45"/>
+      <c r="AD6" s="45"/>
+      <c r="AE6" s="45"/>
+      <c r="AF6" s="45"/>
+      <c r="AG6" s="45"/>
+      <c r="AH6" s="45"/>
+      <c r="AK6" s="45"/>
+      <c r="AN6" s="45"/>
+      <c r="AO6" s="45"/>
+      <c r="AP6" s="45"/>
+      <c r="AQ6" s="45"/>
+      <c r="AR6" s="45"/>
+      <c r="AS6" s="45"/>
+      <c r="AT6" s="45"/>
+      <c r="AU6" s="45"/>
+      <c r="AV6" s="45"/>
+      <c r="AW6" s="45"/>
+      <c r="AX6" s="45"/>
+      <c r="AY6" s="45"/>
+      <c r="AZ6" s="45"/>
+      <c r="BA6" s="45"/>
+      <c r="BB6" s="45"/>
+      <c r="BC6" s="45"/>
+      <c r="BD6" s="45"/>
+      <c r="BE6" s="45"/>
+      <c r="BF6" s="45"/>
+      <c r="BG6" s="45"/>
+      <c r="BH6" s="45"/>
+      <c r="BI6" s="45"/>
+      <c r="BJ6" s="45"/>
+      <c r="BK6" s="45"/>
+      <c r="BL6" s="45"/>
+      <c r="BM6" s="45"/>
+      <c r="BN6" s="45"/>
+      <c r="BO6" s="45"/>
     </row>
     <row r="7">
       <c r="A7" s="35">
         <v>2.0</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>155</v>
+      <c r="B7" s="44" t="s">
+        <v>161</v>
       </c>
       <c r="C7" s="37"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -1670,7 +1914,7 @@
       <c r="AI7" s="14"/>
       <c r="AJ7" s="14"/>
       <c r="AK7" s="15"/>
-      <c r="AN7" s="43"/>
+      <c r="AN7" s="45"/>
       <c r="AO7" s="15"/>
       <c r="AP7" s="15"/>
       <c r="AQ7" s="15"/>
@@ -1700,197 +1944,203 @@
       <c r="BO7" s="15"/>
     </row>
     <row r="8">
-      <c r="A8" s="44">
+      <c r="A8" s="46">
         <v>3.0</v>
       </c>
-      <c r="B8" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="48">
+      <c r="B8" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="50">
         <v>1800.0</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="M8" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="N8" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="O8" s="50">
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="M8" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="N8" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="O8" s="52">
         <v>211.0</v>
       </c>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="50">
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="52">
         <v>217.0</v>
       </c>
-      <c r="T8" s="51"/>
-      <c r="U8" s="50">
+      <c r="T8" s="53"/>
+      <c r="U8" s="52">
         <v>130.0</v>
       </c>
-      <c r="V8" s="51"/>
-      <c r="W8" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="50">
+      <c r="V8" s="53"/>
+      <c r="W8" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="X8" s="53"/>
+      <c r="Y8" s="52">
         <v>536.0</v>
       </c>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="51"/>
-      <c r="AC8" s="50">
+      <c r="Z8" s="53"/>
+      <c r="AA8" s="53"/>
+      <c r="AB8" s="53"/>
+      <c r="AC8" s="52">
         <v>217.0</v>
       </c>
-      <c r="AD8" s="51"/>
-      <c r="AE8" s="50">
+      <c r="AD8" s="53"/>
+      <c r="AE8" s="52">
         <v>130.0</v>
       </c>
-      <c r="AF8" s="51"/>
-      <c r="AG8" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="52"/>
-      <c r="AJ8" s="52"/>
-      <c r="AK8" s="51"/>
-      <c r="AN8" s="43"/>
-      <c r="AO8" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="AP8" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="AQ8" s="48" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR8" s="50">
+      <c r="AF8" s="53"/>
+      <c r="AG8" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="AH8" s="53"/>
+      <c r="AI8" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ8" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="AK8" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="AN8" s="45"/>
+      <c r="AO8" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP8" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ8" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR8" s="52">
         <v>6830.0</v>
       </c>
-      <c r="AS8" s="51"/>
-      <c r="AT8" s="51"/>
-      <c r="AU8" s="51"/>
-      <c r="AV8" s="50">
+      <c r="AS8" s="53"/>
+      <c r="AT8" s="53"/>
+      <c r="AU8" s="53"/>
+      <c r="AV8" s="52">
         <v>7161.0</v>
       </c>
-      <c r="AW8" s="51"/>
-      <c r="AX8" s="51"/>
-      <c r="AY8" s="51"/>
-      <c r="AZ8" s="50">
+      <c r="AW8" s="53"/>
+      <c r="AX8" s="53"/>
+      <c r="AY8" s="53"/>
+      <c r="AZ8" s="52">
         <v>7822.0</v>
       </c>
-      <c r="BA8" s="51"/>
-      <c r="BB8" s="51"/>
-      <c r="BC8" s="51"/>
-      <c r="BD8" s="50">
+      <c r="BA8" s="53"/>
+      <c r="BB8" s="53"/>
+      <c r="BC8" s="53"/>
+      <c r="BD8" s="52">
         <v>8813.0</v>
       </c>
-      <c r="BE8" s="51"/>
-      <c r="BF8" s="51"/>
-      <c r="BG8" s="51"/>
-      <c r="BH8" s="50">
+      <c r="BE8" s="53"/>
+      <c r="BF8" s="53"/>
+      <c r="BG8" s="53"/>
+      <c r="BH8" s="52">
         <v>8924.0</v>
       </c>
-      <c r="BI8" s="51"/>
-      <c r="BJ8" s="51"/>
-      <c r="BK8" s="51"/>
-      <c r="BL8" s="50">
+      <c r="BI8" s="53"/>
+      <c r="BJ8" s="53"/>
+      <c r="BK8" s="53"/>
+      <c r="BL8" s="52">
         <v>6279.0</v>
       </c>
-      <c r="BM8" s="51"/>
-      <c r="BN8" s="51"/>
-      <c r="BO8" s="51"/>
+      <c r="BM8" s="53"/>
+      <c r="BN8" s="53"/>
+      <c r="BO8" s="53"/>
     </row>
     <row r="9">
-      <c r="A9" s="44">
+      <c r="A9" s="46">
         <v>4.0</v>
       </c>
-      <c r="B9" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="43"/>
-      <c r="Z9" s="43"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="43"/>
-      <c r="AC9" s="43"/>
-      <c r="AD9" s="43"/>
-      <c r="AE9" s="43"/>
-      <c r="AF9" s="43"/>
-      <c r="AG9" s="43"/>
-      <c r="AH9" s="43"/>
-      <c r="AK9" s="43"/>
-      <c r="AN9" s="43"/>
-      <c r="AO9" s="43"/>
-      <c r="AP9" s="43"/>
-      <c r="AQ9" s="43"/>
-      <c r="AR9" s="43"/>
-      <c r="AS9" s="43"/>
-      <c r="AT9" s="43"/>
-      <c r="AU9" s="43"/>
-      <c r="AV9" s="43"/>
-      <c r="AW9" s="43"/>
-      <c r="AX9" s="43"/>
-      <c r="AY9" s="43"/>
-      <c r="AZ9" s="43"/>
-      <c r="BA9" s="43"/>
-      <c r="BB9" s="43"/>
-      <c r="BC9" s="43"/>
-      <c r="BD9" s="43"/>
-      <c r="BE9" s="43"/>
-      <c r="BF9" s="43"/>
-      <c r="BG9" s="43"/>
-      <c r="BH9" s="43"/>
-      <c r="BI9" s="43"/>
-      <c r="BJ9" s="43"/>
-      <c r="BK9" s="43"/>
-      <c r="BL9" s="43"/>
-      <c r="BM9" s="43"/>
-      <c r="BN9" s="43"/>
-      <c r="BO9" s="43"/>
+      <c r="B9" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="45"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="45"/>
+      <c r="U9" s="45"/>
+      <c r="V9" s="45"/>
+      <c r="W9" s="45"/>
+      <c r="X9" s="45"/>
+      <c r="Y9" s="45"/>
+      <c r="Z9" s="45"/>
+      <c r="AA9" s="45"/>
+      <c r="AB9" s="45"/>
+      <c r="AC9" s="45"/>
+      <c r="AD9" s="45"/>
+      <c r="AE9" s="45"/>
+      <c r="AF9" s="45"/>
+      <c r="AG9" s="45"/>
+      <c r="AH9" s="45"/>
+      <c r="AK9" s="45"/>
+      <c r="AN9" s="45"/>
+      <c r="AO9" s="45"/>
+      <c r="AP9" s="45"/>
+      <c r="AQ9" s="45"/>
+      <c r="AR9" s="45"/>
+      <c r="AS9" s="45"/>
+      <c r="AT9" s="45"/>
+      <c r="AU9" s="45"/>
+      <c r="AV9" s="45"/>
+      <c r="AW9" s="45"/>
+      <c r="AX9" s="45"/>
+      <c r="AY9" s="45"/>
+      <c r="AZ9" s="45"/>
+      <c r="BA9" s="45"/>
+      <c r="BB9" s="45"/>
+      <c r="BC9" s="45"/>
+      <c r="BD9" s="45"/>
+      <c r="BE9" s="45"/>
+      <c r="BF9" s="45"/>
+      <c r="BG9" s="45"/>
+      <c r="BH9" s="45"/>
+      <c r="BI9" s="45"/>
+      <c r="BJ9" s="45"/>
+      <c r="BK9" s="45"/>
+      <c r="BL9" s="45"/>
+      <c r="BM9" s="45"/>
+      <c r="BN9" s="45"/>
+      <c r="BO9" s="45"/>
     </row>
     <row r="10">
-      <c r="A10" s="44">
+      <c r="A10" s="46">
         <v>4.0</v>
       </c>
-      <c r="B10" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10" s="46"/>
+      <c r="B10" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="48"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -1922,8 +2172,8 @@
       <c r="AF10" s="15"/>
       <c r="AG10" s="15"/>
       <c r="AH10" s="15"/>
-      <c r="AK10" s="43"/>
-      <c r="AN10" s="43"/>
+      <c r="AK10" s="45"/>
+      <c r="AN10" s="45"/>
       <c r="AO10" s="15"/>
       <c r="AP10" s="15"/>
       <c r="AQ10" s="15"/>
@@ -1952,10 +2202,576 @@
       <c r="BN10" s="15"/>
       <c r="BO10" s="15"/>
     </row>
+    <row r="11">
+      <c r="A11" s="56">
+        <v>5.0</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G11" s="57" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="I11" s="58">
+        <v>1700.0</v>
+      </c>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="M11" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="N11" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="O11" s="39">
+        <v>192.0</v>
+      </c>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="39">
+        <v>217.0</v>
+      </c>
+      <c r="T11" s="40"/>
+      <c r="U11" s="39">
+        <v>130.0</v>
+      </c>
+      <c r="V11" s="40"/>
+      <c r="W11" s="58" t="s">
+        <v>185</v>
+      </c>
+      <c r="X11" s="40"/>
+      <c r="Y11" s="39">
+        <v>488.0</v>
+      </c>
+      <c r="Z11" s="40"/>
+      <c r="AA11" s="40"/>
+      <c r="AB11" s="40"/>
+      <c r="AC11" s="39">
+        <v>450.0</v>
+      </c>
+      <c r="AD11" s="40"/>
+      <c r="AE11" s="39">
+        <v>130.0</v>
+      </c>
+      <c r="AF11" s="40"/>
+      <c r="AG11" s="58" t="s">
+        <v>185</v>
+      </c>
+      <c r="AH11" s="40"/>
+      <c r="AI11" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ11" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK11" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="AL11" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="AM11" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="AN11" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="AO11" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="AP11" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="AQ11" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="AR11" s="39">
+        <v>5702.0</v>
+      </c>
+      <c r="AS11" s="40"/>
+      <c r="AT11" s="40"/>
+      <c r="AU11" s="40"/>
+      <c r="AV11" s="39">
+        <v>6032.0</v>
+      </c>
+      <c r="AW11" s="40"/>
+      <c r="AX11" s="40"/>
+      <c r="AY11" s="40"/>
+      <c r="AZ11" s="39">
+        <v>6692.0</v>
+      </c>
+      <c r="BA11" s="40"/>
+      <c r="BB11" s="40"/>
+      <c r="BC11" s="40"/>
+      <c r="BD11" s="39">
+        <v>7685.0</v>
+      </c>
+      <c r="BE11" s="40"/>
+      <c r="BF11" s="40"/>
+      <c r="BG11" s="40"/>
+      <c r="BH11" s="39">
+        <v>7794.0</v>
+      </c>
+      <c r="BI11" s="40"/>
+      <c r="BJ11" s="40"/>
+      <c r="BK11" s="40"/>
+      <c r="BL11" s="39">
+        <v>5151.0</v>
+      </c>
+      <c r="BM11" s="40"/>
+      <c r="BN11" s="40"/>
+      <c r="BO11" s="40"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="56">
+        <v>6.0</v>
+      </c>
+      <c r="B12" s="61" t="s">
+        <v>192</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="45"/>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="45"/>
+      <c r="AA12" s="45"/>
+      <c r="AB12" s="45"/>
+      <c r="AC12" s="45"/>
+      <c r="AD12" s="45"/>
+      <c r="AE12" s="45"/>
+      <c r="AF12" s="45"/>
+      <c r="AG12" s="45"/>
+      <c r="AH12" s="45"/>
+      <c r="AK12" s="45"/>
+      <c r="AN12" s="45"/>
+      <c r="AO12" s="45"/>
+      <c r="AP12" s="45"/>
+      <c r="AQ12" s="45"/>
+      <c r="AR12" s="45"/>
+      <c r="AS12" s="40"/>
+      <c r="AT12" s="40"/>
+      <c r="AU12" s="40"/>
+      <c r="AV12" s="45"/>
+      <c r="AW12" s="40"/>
+      <c r="AX12" s="40"/>
+      <c r="AY12" s="40"/>
+      <c r="AZ12" s="45"/>
+      <c r="BA12" s="40"/>
+      <c r="BB12" s="40"/>
+      <c r="BC12" s="40"/>
+      <c r="BD12" s="45"/>
+      <c r="BE12" s="40"/>
+      <c r="BF12" s="40"/>
+      <c r="BG12" s="40"/>
+      <c r="BH12" s="45"/>
+      <c r="BI12" s="40"/>
+      <c r="BJ12" s="40"/>
+      <c r="BK12" s="40"/>
+      <c r="BL12" s="45"/>
+      <c r="BM12" s="40"/>
+      <c r="BN12" s="40"/>
+      <c r="BO12" s="40"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="62">
+        <v>6.0</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="48"/>
+      <c r="D13" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="64">
+        <v>1900.0</v>
+      </c>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="M13" s="63" t="s">
+        <v>195</v>
+      </c>
+      <c r="N13" s="63" t="s">
+        <v>196</v>
+      </c>
+      <c r="O13" s="52">
+        <v>211.0</v>
+      </c>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="52">
+        <v>217.0</v>
+      </c>
+      <c r="T13" s="51"/>
+      <c r="U13" s="52">
+        <v>130.0</v>
+      </c>
+      <c r="V13" s="51"/>
+      <c r="W13" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="X13" s="51"/>
+      <c r="Y13" s="52">
+        <v>536.0</v>
+      </c>
+      <c r="Z13" s="51"/>
+      <c r="AA13" s="51"/>
+      <c r="AB13" s="51"/>
+      <c r="AC13" s="52">
+        <v>217.0</v>
+      </c>
+      <c r="AD13" s="51"/>
+      <c r="AE13" s="52">
+        <v>130.0</v>
+      </c>
+      <c r="AF13" s="51"/>
+      <c r="AG13" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH13" s="51"/>
+      <c r="AI13" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ13" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="AK13" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="AN13" s="45"/>
+      <c r="AO13" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP13" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ13" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR13" s="52">
+        <v>6830.0</v>
+      </c>
+      <c r="AS13" s="37"/>
+      <c r="AT13" s="37"/>
+      <c r="AU13" s="37"/>
+      <c r="AV13" s="52">
+        <v>7161.0</v>
+      </c>
+      <c r="AW13" s="37"/>
+      <c r="AX13" s="37"/>
+      <c r="AY13" s="37"/>
+      <c r="AZ13" s="52">
+        <v>7822.0</v>
+      </c>
+      <c r="BA13" s="37"/>
+      <c r="BB13" s="37"/>
+      <c r="BC13" s="37"/>
+      <c r="BD13" s="52">
+        <v>8813.0</v>
+      </c>
+      <c r="BE13" s="37"/>
+      <c r="BF13" s="37"/>
+      <c r="BG13" s="37"/>
+      <c r="BH13" s="52">
+        <v>8924.0</v>
+      </c>
+      <c r="BI13" s="37"/>
+      <c r="BJ13" s="37"/>
+      <c r="BK13" s="37"/>
+      <c r="BL13" s="52">
+        <v>6279.0</v>
+      </c>
+      <c r="BM13" s="37"/>
+      <c r="BN13" s="37"/>
+      <c r="BO13" s="37"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="62">
+        <v>7.0</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="48"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="51"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="45"/>
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="45"/>
+      <c r="AF14" s="51"/>
+      <c r="AG14" s="45"/>
+      <c r="AH14" s="51"/>
+      <c r="AK14" s="45"/>
+      <c r="AN14" s="45"/>
+      <c r="AO14" s="45"/>
+      <c r="AP14" s="45"/>
+      <c r="AQ14" s="45"/>
+      <c r="AR14" s="45"/>
+      <c r="AS14" s="53"/>
+      <c r="AT14" s="53"/>
+      <c r="AU14" s="53"/>
+      <c r="AV14" s="45"/>
+      <c r="AW14" s="53"/>
+      <c r="AX14" s="53"/>
+      <c r="AY14" s="53"/>
+      <c r="AZ14" s="45"/>
+      <c r="BA14" s="53"/>
+      <c r="BB14" s="53"/>
+      <c r="BC14" s="53"/>
+      <c r="BD14" s="45"/>
+      <c r="BE14" s="53"/>
+      <c r="BF14" s="53"/>
+      <c r="BG14" s="53"/>
+      <c r="BH14" s="45"/>
+      <c r="BI14" s="53"/>
+      <c r="BJ14" s="53"/>
+      <c r="BK14" s="53"/>
+      <c r="BL14" s="45"/>
+      <c r="BM14" s="53"/>
+      <c r="BN14" s="53"/>
+      <c r="BO14" s="53"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="62">
+        <v>8.0</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="48"/>
+      <c r="D15" s="63" t="s">
+        <v>201</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="68">
+        <v>2100.0</v>
+      </c>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="70" t="s">
+        <v>202</v>
+      </c>
+      <c r="M15" s="70" t="s">
+        <v>203</v>
+      </c>
+      <c r="N15" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="O15" s="68">
+        <v>230.0</v>
+      </c>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="68">
+        <v>217.0</v>
+      </c>
+      <c r="T15" s="69"/>
+      <c r="U15" s="68">
+        <v>130.0</v>
+      </c>
+      <c r="V15" s="69"/>
+      <c r="W15" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="X15" s="69"/>
+      <c r="Y15" s="68">
+        <v>636.0</v>
+      </c>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="72">
+        <v>217.0</v>
+      </c>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="72">
+        <v>130.0</v>
+      </c>
+      <c r="AF15" s="69"/>
+      <c r="AG15" s="68" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="73" t="s">
+        <v>206</v>
+      </c>
+      <c r="AJ15" s="73" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK15" s="74" t="s">
+        <v>208</v>
+      </c>
+      <c r="AN15" s="45"/>
+      <c r="AO15" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP15" s="72" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ15" s="72" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR15" s="72">
+        <v>6830.0</v>
+      </c>
+      <c r="AS15" s="69"/>
+      <c r="AT15" s="69"/>
+      <c r="AU15" s="69"/>
+      <c r="AV15" s="72">
+        <v>7161.0</v>
+      </c>
+      <c r="AW15" s="69"/>
+      <c r="AX15" s="69"/>
+      <c r="AY15" s="69"/>
+      <c r="AZ15" s="72">
+        <v>7822.0</v>
+      </c>
+      <c r="BA15" s="69"/>
+      <c r="BB15" s="69"/>
+      <c r="BC15" s="69"/>
+      <c r="BD15" s="72">
+        <v>8813.0</v>
+      </c>
+      <c r="BE15" s="69"/>
+      <c r="BF15" s="69"/>
+      <c r="BG15" s="69"/>
+      <c r="BH15" s="72">
+        <v>8924.0</v>
+      </c>
+      <c r="BI15" s="69"/>
+      <c r="BJ15" s="69"/>
+      <c r="BK15" s="69"/>
+      <c r="BL15" s="72">
+        <v>6279.0</v>
+      </c>
+      <c r="BM15" s="69"/>
+      <c r="BN15" s="69"/>
+      <c r="BO15" s="69"/>
+    </row>
   </sheetData>
-  <mergeCells count="130">
+  <mergeCells count="201">
+    <mergeCell ref="AG11:AG12"/>
+    <mergeCell ref="AH11:AH12"/>
+    <mergeCell ref="AF8:AF10"/>
+    <mergeCell ref="AG8:AG10"/>
+    <mergeCell ref="AK11:AK12"/>
+    <mergeCell ref="AJ11:AJ12"/>
+    <mergeCell ref="AI13:AI14"/>
+    <mergeCell ref="AJ13:AJ14"/>
+    <mergeCell ref="AK13:AK14"/>
+    <mergeCell ref="AL11:AL15"/>
+    <mergeCell ref="AF11:AF12"/>
+    <mergeCell ref="AG13:AG14"/>
+    <mergeCell ref="AI11:AI12"/>
+    <mergeCell ref="AJ8:AJ10"/>
+    <mergeCell ref="AK8:AK10"/>
+    <mergeCell ref="AF5:AF7"/>
+    <mergeCell ref="AG5:AG7"/>
+    <mergeCell ref="AH5:AH7"/>
+    <mergeCell ref="AI5:AI7"/>
+    <mergeCell ref="AK5:AK7"/>
+    <mergeCell ref="AJ5:AJ7"/>
+    <mergeCell ref="AL5:AL10"/>
+    <mergeCell ref="AH8:AH10"/>
+    <mergeCell ref="AI8:AI10"/>
+    <mergeCell ref="AM5:AM10"/>
+    <mergeCell ref="AN5:AN10"/>
+    <mergeCell ref="AO5:AO7"/>
+    <mergeCell ref="AP5:AP7"/>
+    <mergeCell ref="AQ5:AQ7"/>
+    <mergeCell ref="AR5:AR7"/>
+    <mergeCell ref="AS5:AS7"/>
+    <mergeCell ref="AR11:AR12"/>
+    <mergeCell ref="AV11:AV12"/>
+    <mergeCell ref="AR13:AR14"/>
+    <mergeCell ref="AV13:AV14"/>
+    <mergeCell ref="AO8:AO10"/>
+    <mergeCell ref="AP8:AP10"/>
+    <mergeCell ref="AO11:AO12"/>
+    <mergeCell ref="AP11:AP12"/>
+    <mergeCell ref="AQ11:AQ12"/>
+    <mergeCell ref="AM11:AM15"/>
+    <mergeCell ref="AN11:AN15"/>
+    <mergeCell ref="AO13:AO14"/>
+    <mergeCell ref="AP13:AP14"/>
+    <mergeCell ref="AQ13:AQ14"/>
     <mergeCell ref="BH5:BH7"/>
     <mergeCell ref="BI5:BI7"/>
+    <mergeCell ref="BH13:BH14"/>
+    <mergeCell ref="BL13:BL14"/>
+    <mergeCell ref="AZ13:AZ14"/>
+    <mergeCell ref="BD13:BD14"/>
     <mergeCell ref="BA5:BA7"/>
     <mergeCell ref="BB5:BB7"/>
     <mergeCell ref="BC5:BC7"/>
@@ -1963,8 +2779,18 @@
     <mergeCell ref="BE5:BE7"/>
     <mergeCell ref="BF5:BF7"/>
     <mergeCell ref="BG5:BG7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N13:N14"/>
     <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I13:I14"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E10"/>
     <mergeCell ref="F5:F10"/>
@@ -1972,6 +2798,12 @@
     <mergeCell ref="H5:H10"/>
     <mergeCell ref="J5:J7"/>
     <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="H11:H15"/>
     <mergeCell ref="J8:J10"/>
     <mergeCell ref="K8:K10"/>
     <mergeCell ref="L8:L10"/>
@@ -1994,6 +2826,21 @@
     <mergeCell ref="U8:U10"/>
     <mergeCell ref="V8:V10"/>
     <mergeCell ref="W8:W10"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="AE11:AE12"/>
+    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="AC11:AC12"/>
+    <mergeCell ref="AD11:AD12"/>
     <mergeCell ref="AL2:AN2"/>
     <mergeCell ref="AR2:BO2"/>
     <mergeCell ref="B2:C2"/>
@@ -2060,30 +2907,21 @@
     <mergeCell ref="BK8:BK10"/>
     <mergeCell ref="BL8:BL10"/>
     <mergeCell ref="BM8:BM10"/>
-    <mergeCell ref="AF8:AF10"/>
-    <mergeCell ref="AG8:AG10"/>
-    <mergeCell ref="AH8:AH10"/>
-    <mergeCell ref="AI8:AI10"/>
-    <mergeCell ref="AJ8:AJ10"/>
-    <mergeCell ref="AK8:AK10"/>
-    <mergeCell ref="AF5:AF7"/>
-    <mergeCell ref="AG5:AG7"/>
-    <mergeCell ref="AH5:AH7"/>
-    <mergeCell ref="AI5:AI7"/>
-    <mergeCell ref="AJ5:AJ7"/>
-    <mergeCell ref="AK5:AK7"/>
-    <mergeCell ref="AL5:AL10"/>
-    <mergeCell ref="AO8:AO10"/>
-    <mergeCell ref="AP8:AP10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="W13:W14"/>
     <mergeCell ref="AQ8:AQ10"/>
     <mergeCell ref="AR8:AR10"/>
-    <mergeCell ref="AM5:AM10"/>
-    <mergeCell ref="AN5:AN10"/>
-    <mergeCell ref="AO5:AO7"/>
-    <mergeCell ref="AP5:AP7"/>
-    <mergeCell ref="AQ5:AQ7"/>
-    <mergeCell ref="AR5:AR7"/>
-    <mergeCell ref="AS5:AS7"/>
+    <mergeCell ref="AZ11:AZ12"/>
+    <mergeCell ref="BH11:BH12"/>
+    <mergeCell ref="BL11:BL12"/>
+    <mergeCell ref="BD11:BD12"/>
+    <mergeCell ref="AC13:AC14"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>